<commit_message>
Update Medical Imaging Interview Record.xlsx
</commit_message>
<xml_diff>
--- a/StateOfPractice/Ao-Notes/Medical Imaging Interview Record.xlsx
+++ b/StateOfPractice/Ao-Notes/Medical Imaging Interview Record.xlsx
@@ -862,13 +862,13 @@
   </sheetPr>
   <dimension ref="A1:AD29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="O7" activeCellId="0" sqref="O7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="C4" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topRight" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.671875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="20.6796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28"/>
   </cols>
@@ -1637,7 +1637,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>149</v>
       </c>
@@ -1694,9 +1694,12 @@
         <v>44319</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>132</v>
+      </c>
+      <c r="E21" s="5" t="n">
+        <v>44320</v>
       </c>
       <c r="I21" s="5" t="n">
         <v>44259</v>
@@ -1713,9 +1716,12 @@
       <c r="AC21" s="2"/>
       <c r="AD21" s="2"/>
     </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
         <v>133</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>44341</v>
       </c>
       <c r="I22" s="5" t="n">
         <v>44266</v>
@@ -1812,12 +1818,12 @@
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10:B10 D10:E10 G10 I10:AD10">
+  <conditionalFormatting sqref="A10:B10 D10:E10 G10 I10:AD10 E21">
     <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>LEN(TRIM(A10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:B11 G11:AD11 D11:E11">
+  <conditionalFormatting sqref="A11:B11 G11:AD11 D11:E11 E22">
     <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>LEN(TRIM(A11))&gt;0</formula>
     </cfRule>
@@ -1842,12 +1848,12 @@
       <formula>LEN(TRIM(C11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A21:B21 G21:AD21 D21:E21">
+  <conditionalFormatting sqref="A21:B21 G21:AD21 D21">
     <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>LEN(TRIM(A21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A22:B22 G22:AD22 D22:E22">
+  <conditionalFormatting sqref="A22:B22 G22:AD22 D22">
     <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>LEN(TRIM(A22))&gt;0</formula>
     </cfRule>
@@ -1862,12 +1868,12 @@
       <formula>LEN(TRIM(F22))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B21:S21">
+  <conditionalFormatting sqref="F21:S21 B21:D21">
     <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
       <formula>LEN(TRIM(B21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B22:S22">
+  <conditionalFormatting sqref="F22:S22 B22:D22">
     <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
       <formula>LEN(TRIM(B22))&gt;0</formula>
     </cfRule>

</xml_diff>